<commit_message>
rename some variables +  add uncertainty calculation
</commit_message>
<xml_diff>
--- a/Data/Raw/MIS_2022_v3_aller_simple.xlsx
+++ b/Data/Raw/MIS_2022_v3_aller_simple.xlsx
@@ -298,7 +298,7 @@
     <t xml:space="preserve">ISSY-LES-MOULINEAUX</t>
   </si>
   <si>
-    <t xml:space="preserve">karlsruhe, bad-Wurtemberg</t>
+    <t xml:space="preserve">karlsruhe</t>
   </si>
   <si>
     <t xml:space="preserve">Metro,Taxi,Train,Location de véhicule</t>
@@ -1180,11 +1180,11 @@
   </sheetPr>
   <dimension ref="A1:K377"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B36" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F46" activeCellId="0" sqref="F46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.37"/>
@@ -1193,7 +1193,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="39.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="25.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.43"/>

</xml_diff>